<commit_message>
update brochure config excels
</commit_message>
<xml_diff>
--- a/brochures/excel/offshore/seapae/AIBT.xlsx
+++ b/brochures/excel/offshore/seapae/AIBT.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zchen\OneDrive - Amadeus Workplace\Desktop\Promotion\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelon\Documents\Code\ViskeeConsultancy\Viskee-Consultancy-Configuration\brochures\excel\offshore\seapae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC104856B95C5AF65BDE58E8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{90B207DE-8914-473F-B25E-1B9621FA0272}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="promotions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -33,45 +32,29 @@
     <t>link</t>
   </si>
   <si>
-    <t>Q2 Promotions Brochure.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/AibtGlobal/Viskee-Consultancy-Configuration/raw/master/promotion/Q2_Promotions_Brochure_1APR-30JUN21_MAR21_APR_01.pdf</t>
-  </si>
-  <si>
-    <t>Courses Fees MARCH 2021 VOL3.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/AibtGlobal/Viskee-Consultancy-Configuration/raw/master/promotion/Courses_Fees-MAR21_03.pdf</t>
-  </si>
-  <si>
-    <t>New SISMIC Region H1 VOL3.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/AibtGlobal/Viskee-Consultancy-Configuration/raw/master/promotion/New_SISMIC_Region_H1_vol3.pdf</t>
-  </si>
-  <si>
-    <t>Non CoE Promotions Brochure 1APR2021-3OJUN2021 VOL1.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/AibtGlobal/Viskee-Consultancy-Configuration/raw/master/promotion/Non-CoE_Promotions_Brochure_1APR2021-3OJUN2021_VOL1.pdf</t>
-  </si>
-  <si>
-    <t>SEAPAE Course Information Brochure Region 2 H1 MAR VOL2.pdf</t>
-  </si>
-  <si>
-    <t>https://github.com/AibtGlobal/Viskee-Consultancy-Configuration/raw/master/promotion/SEAPAE_Course_Information_Brochure_Region_2_H1_MAR_VOL2.pdf</t>
+    <t>AIBT Courses Fees 2021.pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/seapae/aibt/AIBT_Courses_Fees_2021_VOL_2.2.pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIBT Region1(SEAPAE) Q4 Promotion.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/Viskee-Consultancy/Viskee-Consultancy-Configuration/raw/master/brochures/pdf/offshore/seapae/aibt/AIBTSEAPAE_Q4_Brochure_1OCT-31DEC21_VOL1.1.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +62,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -101,16 +99,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,20 +389,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="135" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,15 +410,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -425,32 +426,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>